<commit_message>
adding the changes and creating the upload for projects file
</commit_message>
<xml_diff>
--- a/assessmentresult.xlsx
+++ b/assessmentresult.xlsx
@@ -416,13 +416,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3.67</v>
       </c>
       <c r="F2" t="n">
         <v>4</v>
       </c>
       <c r="G2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -443,13 +443,13 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3.67</v>
       </c>
       <c r="F3" t="n">
         <v>4</v>
       </c>
       <c r="G3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -470,13 +470,13 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3.67</v>
       </c>
       <c r="F4" t="n">
         <v>4</v>
       </c>
       <c r="G4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -497,13 +497,13 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3.67</v>
       </c>
       <c r="F5" t="n">
         <v>4</v>
       </c>
       <c r="G5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -524,13 +524,13 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3.67</v>
       </c>
       <c r="F6" t="n">
         <v>4</v>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing bugs and making modification to the visuals
</commit_message>
<xml_diff>
--- a/assessmentresult.xlsx
+++ b/assessmentresult.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -400,55 +400,67 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jenna</t>
+          <t>Yvan</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>McConnell</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" t="n">
-        <v>4</v>
-      </c>
-      <c r="F2" t="n">
-        <v>4</v>
+          <t>Labiche</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Saundra</t>
+          <t>Jenna</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Warmington</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" t="n">
-        <v>3</v>
-      </c>
-      <c r="F3" t="n">
-        <v>3</v>
+          <t>McConnell</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -460,68 +472,194 @@
           <t>Poll</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" t="n">
-        <v>3</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Darlene</t>
+          <t>Saundra</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Hebert</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F5" t="n">
-        <v>3</v>
+          <t>Warmington</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Erica</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>East</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>15</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jerry </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Buburuz</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>16</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Daren </t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Russ</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>17</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">kong </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Chiv</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>18</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>Ishdeep</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Singh</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
+      <c r="D10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the index and the download file
</commit_message>
<xml_diff>
--- a/assessmentresult.xlsx
+++ b/assessmentresult.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,117 +369,239 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>userId</t>
+          <t>Indicator</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>firstName</t>
+          <t>Level 1: Beginning</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>lastName</t>
+          <t>Level 2: Developing</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>6.1 Personal and group time management</t>
+          <t>Level 3: Accomplished</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>6.2 Group culture, group dynamics</t>
+          <t>Level 4: Exemplary</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>6.3 Leadership: initiative and mentoring, areas of expertise, and interdisciplinary teams</t>
+          <t>Yvan Labiche</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Jenna McConnell</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Jennifer Poll</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Saundra Warmington</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Erica East</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Jerry  Buburuz</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Daren  Russ</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>kong  Chiv</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Ishdeep Singh</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>10</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>6.1 Personal and group time management</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Yvan</t>
+          <t>Deadlines often missed. Several projects or assignments appear hurried or inadequately addressed. No evidence of time management planning.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Labiche</t>
+          <t>Some deadlines missed. Some tasks or assignments appear hurried or inadequately addressed. Some evidence of time management planning.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>No important deadlines missed. Few tasks or assignments appear hurried or inadequately addressed. Good time management planning.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>No deadlines missed. Tasks and assignments always excellently prepared and presented. Tasks occasionally completed ahead of schedule. Leadership in time planning.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>11</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>6.2 Group culture, group dynamics</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jenna</t>
+          <t>Not dependable. Little or no trust from teammates. Dishonest or evasive interactions with teammates. Poor conflict resolution.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>McConnell</t>
+          <t>Usually dependable and trusted by teammates. Mostly ethical behavior towards project and teammates. Minor conflicts.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Dependable and trusted by teammates. Ethical open interactions with teammates. Good conflict resolution.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Dependable and trusted by teammates. Ethical and open interactions with teammates. Leads team in ethical and responsive behavior. Leadership in conflict resolution.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>12</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>6.3 Leadership: initiative and mentoring, areas of expertise, and interdisciplinary teams</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jennifer</t>
+          <t>No initiative. No effort to mentor group members or take ownership of an area of expertise.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Poll</t>
+          <t>Some initiative. Some effort to mentor group members and take ownership of an area of expertise.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Good initiative and self-motivation. Regular effort to mentor group members. Clear command of an area of expertise.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Self-motivated, with regular demonstration of initiative. Constructively directs other team members and helps them to improve at their tasks. High degree of knowledge in an area of expertise.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -487,178 +609,42 @@
           <t>NA</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>13</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Saundra</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Warmington</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>14</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Erica</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>East</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>15</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Jerry </t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Buburuz</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>16</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Daren </t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Russ</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>17</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">kong </t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Chiv</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>18</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Ishdeep</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Singh</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>4</v>
-      </c>
-      <c r="E10" t="n">
-        <v>4</v>
-      </c>
-      <c r="F10" t="n">
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changing the bugs discovered by jenna, changing the download format of the file
</commit_message>
<xml_diff>
--- a/assessmentresult.xlsx
+++ b/assessmentresult.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,169 +369,81 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Indicator</t>
+          <t>StudentId</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Level 1: Beginning</t>
+          <t>LastName</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Level 2: Developing</t>
+          <t>FirstName</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Level 3: Accomplished</t>
+          <t>GA 6.1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Level 4: Exemplary</t>
+          <t>GA 6.2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Yvan Labiche</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Jenna McConnell</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Jennifer Poll</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Saundra Warmington</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Erica East</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Jerry  Buburuz</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Daren  Russ</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>kong  Chiv</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Ishdeep Singh</t>
+          <t>GA 6.3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>6.1 Personal and group time management</t>
-        </is>
+      <c r="A2" t="n">
+        <v>18</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Deadlines often missed. Several projects or assignments appear hurried or inadequately addressed. No evidence of time management planning.</t>
+          <t>Singh</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Some deadlines missed. Some tasks or assignments appear hurried or inadequately addressed. Some evidence of time management planning.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>No important deadlines missed. Few tasks or assignments appear hurried or inadequately addressed. Good time management planning.</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>No deadlines missed. Tasks and assignments always excellently prepared and presented. Tasks occasionally completed ahead of schedule. Leadership in time planning.</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="N2" t="n">
+          <t>Ishdeep</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>4</v>
       </c>
+      <c r="E2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>6.2 Group culture, group dynamics</t>
-        </is>
+      <c r="A3" t="n">
+        <v>10</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Not dependable. Little or no trust from teammates. Dishonest or evasive interactions with teammates. Poor conflict resolution.</t>
+          <t>Labiche</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Usually dependable and trusted by teammates. Mostly ethical behavior towards project and teammates. Minor conflicts.</t>
+          <t>Yvan</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Dependable and trusted by teammates. Ethical open interactions with teammates. Good conflict resolution.</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Dependable and trusted by teammates. Ethical and open interactions with teammates. Leads team in ethical and responsive behavior. Leadership in conflict resolution.</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -539,69 +451,29 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="N3" t="n">
-        <v>4</v>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>6.3 Leadership: initiative and mentoring, areas of expertise, and interdisciplinary teams</t>
-        </is>
+      <c r="A4" t="n">
+        <v>11</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>No initiative. No effort to mentor group members or take ownership of an area of expertise.</t>
+          <t>McConnell</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Some initiative. Some effort to mentor group members and take ownership of an area of expertise.</t>
+          <t>Jenna</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Good initiative and self-motivation. Regular effort to mentor group members. Clear command of an area of expertise.</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Self-motivated, with regular demonstration of initiative. Constructively directs other team members and helps them to improve at their tasks. High degree of knowledge in an area of expertise.</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -609,43 +481,185 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="N4" t="n">
-        <v>4</v>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>12</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Poll</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Jennifer</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>13</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Warmington</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Saundra</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>14</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>East</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Erica</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>15</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Buburuz</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jerry </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>16</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Russ</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Daren </t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>17</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Chiv</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">kong </t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding the faceligt to the uploaders and the user access role
</commit_message>
<xml_diff>
--- a/assessmentresult.xlsx
+++ b/assessmentresult.xlsx
@@ -369,7 +369,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>StudentId</t>
+          <t>StudentId/GA</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -413,13 +413,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
adding the read me file
</commit_message>
<xml_diff>
--- a/assessmentresult.xlsx
+++ b/assessmentresult.xlsx
@@ -400,70 +400,64 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Singh</t>
+          <t>Russ</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ishdeep</t>
+          <t xml:space="preserve">Daren </t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Labiche</t>
+          <t>Singh</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Yvan</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
+          <t>Ishdeep</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>McConnell</t>
+          <t>Labiche</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jenna</t>
+          <t>Yvan</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -484,16 +478,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Poll</t>
+          <t>McConnell</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Jennifer</t>
+          <t>Jenna</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -514,16 +508,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Warmington</t>
+          <t>Poll</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Saundra</t>
+          <t>Jennifer</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -544,16 +538,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>East</t>
+          <t>Warmington</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Erica</t>
+          <t>Saundra</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -574,16 +568,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Buburuz</t>
+          <t>East</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jerry </t>
+          <t>Erica</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -604,16 +598,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Russ</t>
+          <t>Buburuz</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Daren </t>
+          <t xml:space="preserve">Jerry </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">

</xml_diff>